<commit_message>
some work on  mapping and R tutorials
</commit_message>
<xml_diff>
--- a/Course_Schedule.xlsx
+++ b/Course_Schedule.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentsecuedu66932-my.sharepoint.com/personal/boltonp17_ecu_edu/Documents/Bioinformatics Workshop May 2020/Course_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C44EFFF2-096E-4916-81B7-772141D05A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{C44EFFF2-096E-4916-81B7-772141D05A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4828830B-1081-4FB9-9F9C-311CD67522C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{9BBDC66C-4308-445A-9908-A0AF7C7880AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Time</t>
   </si>
   <si>
-    <t>Monday</t>
-  </si>
-  <si>
     <t>Tuesday</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Student Pairs</t>
   </si>
   <si>
-    <t>ECU Student + Tahlia Hood-Broadwright (UNCCH)</t>
-  </si>
-  <si>
     <t>Kyle Adams (UNCA) + Maxfield Adair Palmer (UNCCH)</t>
   </si>
   <si>
@@ -127,6 +121,15 @@
   </si>
   <si>
     <t>Independent Project Presentations</t>
+  </si>
+  <si>
+    <t>Monday 7th December</t>
+  </si>
+  <si>
+    <t>Monday 14th</t>
+  </si>
+  <si>
+    <t>Sarah Akers (ECU)  + Tahlia Hood-Broadwright (UNCCH)</t>
   </si>
 </sst>
 </file>
@@ -306,9 +309,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -317,13 +317,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -335,59 +351,46 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -707,7 +710,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,232 +727,232 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
+        <v>9</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
+        <v>10</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
+        <v>11</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
-        <v>9</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="C4" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>12</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>13</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="25"/>
+    </row>
+    <row r="7" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <v>14</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="4" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>15</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="29"/>
+      <c r="L8" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="33"/>
-    </row>
-    <row r="3" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
-        <v>10</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="34"/>
-    </row>
-    <row r="4" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
-        <v>11</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="34"/>
-    </row>
-    <row r="5" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="D9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="34"/>
-    </row>
-    <row r="6" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
-        <v>13</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="34"/>
-    </row>
-    <row r="7" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
-        <v>14</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="35"/>
-    </row>
-    <row r="8" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
-        <v>15</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="27"/>
-      <c r="L8" s="31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="32"/>
+      <c r="E9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="32"/>
+      <c r="H9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="23"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -957,50 +960,44 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="30" t="s">
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>17</v>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J3:J7"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L2:L7"/>
-    <mergeCell ref="K2:K8"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="G2:G9"/>
@@ -1008,6 +1005,12 @@
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="F2:F8"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="L2:L7"/>
+    <mergeCell ref="K2:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
error correct plus popgen tutorial
</commit_message>
<xml_diff>
--- a/Course_Schedule.xlsx
+++ b/Course_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentsecuedu66932-my.sharepoint.com/personal/boltonp17_ecu_edu/Documents/Bioinformatics Workshop May 2020/Course_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="307" documentId="8_{C44EFFF2-096E-4916-81B7-772141D05A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{973594C3-C3A8-4F77-8D85-3B403BA9BC8D}"/>
+  <xr:revisionPtr revIDLastSave="311" documentId="8_{C44EFFF2-096E-4916-81B7-772141D05A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54B4BFF8-6878-4605-A423-4C04B055AAF4}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BBDC66C-4308-445A-9908-A0AF7C7880AD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="82">
   <si>
     <t>Time</t>
   </si>
@@ -218,13 +218,7 @@
     </r>
   </si>
   <si>
-    <t>Student Led Paper Discussion: Max</t>
-  </si>
-  <si>
     <t>Student Led Paper Discussion: Sarah</t>
-  </si>
-  <si>
-    <t>Student Led Paper Discussion: ??</t>
   </si>
   <si>
     <t>Cody Sorrell</t>
@@ -380,6 +374,9 @@
   </si>
   <si>
     <t>Sarah 1545</t>
+  </si>
+  <si>
+    <t>Student Led Paper Discussion: Sue</t>
   </si>
 </sst>
 </file>
@@ -623,9 +620,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -710,6 +704,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1076,7 +1073,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,7 +1091,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1106,7 +1103,7 @@
       <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1132,72 +1129,72 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>9</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="4"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="46"/>
       <c r="L2" s="43"/>
     </row>
     <row r="3" spans="1:12" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>10</v>
       </c>
       <c r="B3" s="51"/>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="35"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="52"/>
       <c r="H3" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K3" s="47"/>
       <c r="L3" s="44"/>
     </row>
     <row r="4" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>11</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="35"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="52"/>
       <c r="H4" s="41"/>
       <c r="I4" s="53" t="s">
@@ -1208,190 +1205,190 @@
       <c r="L4" s="44"/>
     </row>
     <row r="5" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>12</v>
       </c>
       <c r="B5" s="49"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="35"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="34"/>
       <c r="G5" s="52"/>
-      <c r="H5" s="31"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="54"/>
       <c r="J5" s="41"/>
       <c r="K5" s="47"/>
       <c r="L5" s="44"/>
     </row>
     <row r="6" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>13</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="35"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="52"/>
-      <c r="H6" s="31"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="54"/>
       <c r="J6" s="41"/>
       <c r="K6" s="47"/>
       <c r="L6" s="44"/>
     </row>
     <row r="7" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>14</v>
       </c>
       <c r="B7" s="49"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="52"/>
-      <c r="H7" s="32"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="55"/>
       <c r="J7" s="42"/>
       <c r="K7" s="47"/>
       <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>15</v>
       </c>
       <c r="B8" s="50"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="52"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="12" t="s">
+      <c r="H8" s="31"/>
+      <c r="I8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K8" s="48"/>
-      <c r="L8" s="39" t="s">
-        <v>65</v>
+      <c r="L8" s="38" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>55</v>
+      <c r="F9" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="G9" s="52"/>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="38" t="s">
-        <v>82</v>
+      <c r="K9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="37" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>17</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="16"/>
+      <c r="E10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
+      <c r="A11" s="17">
         <v>18</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="33"/>
-      <c r="I11" s="16"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="32"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
+      <c r="A12" s="17">
         <v>19</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="33"/>
-      <c r="I12" s="16"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="32"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="18">
+      <c r="A13" s="17">
         <v>20</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="22"/>
-      <c r="I13" s="16"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="21"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="16"/>
-      <c r="I14" s="16"/>
+      <c r="C14" s="15"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="15"/>
+      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="15"/>
+      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D21" s="15"/>
+      <c r="D21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1425,58 +1422,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1560,7 +1557,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>46</v>
@@ -1574,13 +1571,13 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1611,10 +1608,10 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1625,13 +1622,13 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>